<commit_message>
Continuando con la memoria...
</commit_message>
<xml_diff>
--- a/submissions/tunning_models/xgboost/Comparacion_Tuneo.xlsx
+++ b/submissions/tunning_models/xgboost/Comparacion_Tuneo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alberto/UCM/Aplicaciones del Big Data en la Empresa/practica/AplicacionesBigDataEmpresa/submissions/tunning_models/xgboost/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C40DAABB-1887-9145-A3F7-ABFB9AE73CB1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B1EDD0B-AA33-A449-BD95-08C6D5C374A2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="500" windowWidth="28040" windowHeight="16340" xr2:uid="{EFEC8A58-7E13-2249-954D-6320AB502327}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="45">
   <si>
     <t>Test</t>
   </si>
@@ -154,6 +154,24 @@
   </si>
   <si>
     <t>600 iter</t>
+  </si>
+  <si>
+    <t>700 iter</t>
+  </si>
+  <si>
+    <t>0.119214</t>
+  </si>
+  <si>
+    <t>0.8253</t>
+  </si>
+  <si>
+    <t>semilla</t>
+  </si>
+  <si>
+    <t>0.8259</t>
+  </si>
+  <si>
+    <t>0.8242</t>
   </si>
 </sst>
 </file>
@@ -505,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF566627-2597-6A48-922B-4C6402147087}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -740,7 +758,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -754,7 +772,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -768,7 +786,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -781,8 +799,14 @@
       <c r="D19" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H19" t="s">
+        <v>42</v>
+      </c>
+      <c r="I19" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -795,8 +819,14 @@
       <c r="D20" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H20">
+        <v>123</v>
+      </c>
+      <c r="I20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -809,8 +839,14 @@
       <c r="D21" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H21">
+        <v>1234</v>
+      </c>
+      <c r="I21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -823,8 +859,14 @@
       <c r="D22" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H22">
+        <v>12345</v>
+      </c>
+      <c r="I22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -837,8 +879,14 @@
       <c r="D23" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H23">
+        <v>123456</v>
+      </c>
+      <c r="I23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -851,8 +899,14 @@
       <c r="D24" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="H24">
+        <v>1244</v>
+      </c>
+      <c r="I24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>32</v>
       </c>
@@ -866,7 +920,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -880,7 +934,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>36</v>
       </c>
@@ -894,7 +948,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>37</v>
       </c>
@@ -909,6 +963,26 @@
       </c>
       <c r="E28" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>41</v>
+      </c>
+      <c r="B29" t="s">
+        <v>4</v>
+      </c>
+      <c r="C29">
+        <v>15</v>
+      </c>
+      <c r="D29" t="s">
+        <v>31</v>
+      </c>
+      <c r="E29" t="s">
+        <v>39</v>
+      </c>
+      <c r="F29" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>